<commit_message>
:hammer: feat(lab3/p2-3)!: Parallel RCL circuit calculations done
</commit_message>
<xml_diff>
--- a/lab3/data/2-3.xlsx
+++ b/lab3/data/2-3.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2-3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2-2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2-4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2-2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>f</t>
   </si>
@@ -373,6 +374,75 @@
   </si>
   <si>
     <t xml:space="preserve">Rk [Ом]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U = 6 В; R1 =17 Ом; Rk = 5 Ом; L = 23,094 мГн; C = 71,454 мкФ; f0 = 365.806 Гц</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Xc</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>Gk</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Bk</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t xml:space="preserve">Номер схемы цепи</t>
@@ -452,7 +522,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -489,6 +562,11 @@
       <sz val="11.000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="7">
@@ -529,7 +607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="64">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -984,6 +1062,182 @@
       </left>
       <right style="thin">
         <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color theme="1"/>
       </right>
       <top style="none"/>
       <bottom style="thin">
@@ -1201,7 +1455,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="119">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1347,100 +1601,208 @@
     <xf fontId="0" fillId="0" borderId="32" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="33" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="33" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="34" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="37" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="38" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="39" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="40" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="41" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="42" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="42" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="43" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="43" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="44" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="45" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="45" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="46" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="46" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="47" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="47" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="48" numFmtId="164" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="47" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="48" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="5" fillId="0" borderId="49" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="34" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="50" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="35" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="51" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="36" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="52" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="37" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="53" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="38" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="54" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="39" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="55" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="5" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="40" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="56" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="41" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="57" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="42" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="58" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="43" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="59" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="44" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="60" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="4" borderId="45" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="4" borderId="61" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="4" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="4" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="4" borderId="46" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="4" borderId="62" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="5" borderId="45" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="5" borderId="61" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="5" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="5" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="5" borderId="46" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="5" borderId="62" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="6" borderId="45" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="6" borderId="61" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="6" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="6" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="6" borderId="46" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="6" borderId="62" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="45" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="61" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="55" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="46" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="62" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="42" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="58" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="47" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="63" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="40" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="56" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5376,6 +5738,1280 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="4.140625"/>
+    <col customWidth="1" min="9" max="9" width="10.8515625"/>
+    <col customWidth="1" min="10" max="10" width="6.8515625"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="14.25">
+      <c r="K2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="52"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="K3" s="53"/>
+      <c r="L3" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="59"/>
+    </row>
+    <row r="4" ht="15">
+      <c r="K4" s="60"/>
+      <c r="L4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="B5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="63"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="65" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="55"/>
+      <c r="S5" s="56"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="66">
+        <f>1/(2*PI()*K6*71.454*10^(-6))</f>
+        <v>60.888883774060908</v>
+      </c>
+      <c r="C6" s="16">
+        <f>2*PI()*K6*23.094*10^(-3)</f>
+        <v>5.3080450885664012</v>
+      </c>
+      <c r="D6" s="16">
+        <f>17/(17^2+B6^2)</f>
+        <v>0.0042537686611719286</v>
+      </c>
+      <c r="E6" s="16">
+        <f>5/(5^2+C6^2)</f>
+        <v>0.09402854311175339</v>
+      </c>
+      <c r="F6" s="16">
+        <f>B6/(17^2+B6^2)</f>
+        <v>0.015235719153637662</v>
+      </c>
+      <c r="G6" s="16">
+        <f>C6/(5^2+C6^2)</f>
+        <v>0.099821549289879338</v>
+      </c>
+      <c r="H6" s="16">
+        <f>E6+D6</f>
+        <v>0.098282311772925318</v>
+      </c>
+      <c r="I6" s="16">
+        <f>G6-F6</f>
+        <v>0.084585830136241671</v>
+      </c>
+      <c r="K6" s="67">
+        <v>36.581000000000003</v>
+      </c>
+      <c r="L6" s="68">
+        <f>DEGREES(ATAN(I6/H6))</f>
+        <v>40.716650859719955</v>
+      </c>
+      <c r="M6" s="69">
+        <f>6*SQRT(H6^2+I6^2)</f>
+        <v>0.7780169129406086</v>
+      </c>
+      <c r="N6" s="70">
+        <f>6/SQRT(5^2+C6^2)</f>
+        <v>0.82280344579044173</v>
+      </c>
+      <c r="O6" s="71">
+        <f>6/SQRT(17^2+B6^2)</f>
+        <v>0.094910382436519752</v>
+      </c>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6" s="72"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" s="16">
+        <f>1/(2*PI()*K7*71.454*10^(-6))</f>
+        <v>30.444858016414788</v>
+      </c>
+      <c r="C7" s="16">
+        <f>2*PI()*K7*23.094*10^(-3)</f>
+        <v>10.615945073251318</v>
+      </c>
+      <c r="D7" s="16">
+        <f>17/(17^2+B7^2)</f>
+        <v>0.013981535067802109</v>
+      </c>
+      <c r="E7" s="16">
+        <f>5/(5^2+C7^2)</f>
+        <v>0.036311271602024874</v>
+      </c>
+      <c r="F7" s="16">
+        <f>B7/(17^2+B7^2)</f>
+        <v>0.025039167646515266</v>
+      </c>
+      <c r="G7" s="16">
+        <f>C7/(5^2+C7^2)</f>
+        <v>0.077095692973401284</v>
+      </c>
+      <c r="H7" s="16">
+        <f>E7+D7</f>
+        <v>0.050292806669826981</v>
+      </c>
+      <c r="I7" s="16">
+        <f>G7-F7</f>
+        <v>0.052056525326886018</v>
+      </c>
+      <c r="K7" s="73">
+        <v>73.161000000000001</v>
+      </c>
+      <c r="L7" s="74">
+        <f>DEGREES(ATAN(I7/H7))</f>
+        <v>45.98724273389638</v>
+      </c>
+      <c r="M7" s="75">
+        <f>6*SQRT(H7^2+I7^2)</f>
+        <v>0.43429590873751445</v>
+      </c>
+      <c r="N7" s="76">
+        <f>6/SQRT(5^2+C7^2)</f>
+        <v>0.51131316776959601</v>
+      </c>
+      <c r="O7" s="77">
+        <f>6/SQRT(17^2+B7^2)</f>
+        <v>0.17206962722737901</v>
+      </c>
+      <c r="P7"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78"/>
+      <c r="S7" s="79"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" s="16">
+        <f>1/(2*PI()*K8*71.454*10^(-6))</f>
+        <v>20.296479536904034</v>
+      </c>
+      <c r="C8" s="16">
+        <f>2*PI()*K8*23.094*10^(-3)</f>
+        <v>15.92399016181772</v>
+      </c>
+      <c r="D8" s="16">
+        <f>17/(17^2+B8^2)</f>
+        <v>0.024252900748784417</v>
+      </c>
+      <c r="E8" s="16">
+        <f>5/(5^2+C8^2)</f>
+        <v>0.017948586889833099</v>
+      </c>
+      <c r="F8" s="16">
+        <f>B8/(17^2+B8^2)</f>
+        <v>0.028955794338721613</v>
+      </c>
+      <c r="G8" s="16">
+        <f>C8/(5^2+C8^2)</f>
+        <v>0.057162624210446558</v>
+      </c>
+      <c r="H8" s="16">
+        <f>E8+D8</f>
+        <v>0.042201487638617516</v>
+      </c>
+      <c r="I8" s="16">
+        <f>G8-F8</f>
+        <v>0.028206829871724945</v>
+      </c>
+      <c r="K8" s="73">
+        <v>109.742</v>
+      </c>
+      <c r="L8" s="74">
+        <f>DEGREES(ATAN(I8/H8))</f>
+        <v>33.758162682342622</v>
+      </c>
+      <c r="M8" s="75">
+        <f>6*SQRT(H8^2+I8^2)</f>
+        <v>0.30456078075105725</v>
+      </c>
+      <c r="N8" s="76">
+        <f>6/SQRT(5^2+C8^2)</f>
+        <v>0.35948550124698819</v>
+      </c>
+      <c r="O8" s="77">
+        <f>6/SQRT(17^2+B8^2)</f>
+        <v>0.22662542650506429</v>
+      </c>
+      <c r="P8"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="79"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" s="16">
+        <f>1/(2*PI()*K9*71.454*10^(-6))</f>
+        <v>15.222429008207394</v>
+      </c>
+      <c r="C9" s="16">
+        <f>2*PI()*K9*23.094*10^(-3)</f>
+        <v>21.231890146502636</v>
+      </c>
+      <c r="D9" s="16">
+        <f>17/(17^2+B9^2)</f>
+        <v>0.032646956993829475</v>
+      </c>
+      <c r="E9" s="16">
+        <f>5/(5^2+C9^2)</f>
+        <v>0.010508768155639185</v>
+      </c>
+      <c r="F9" s="16">
+        <f>B9/(17^2+B9^2)</f>
+        <v>0.029233293245445238</v>
+      </c>
+      <c r="G9" s="16">
+        <f>C9/(5^2+C9^2)</f>
+        <v>0.044624202211119256</v>
+      </c>
+      <c r="H9" s="16">
+        <f>E9+D9</f>
+        <v>0.043155725149468659</v>
+      </c>
+      <c r="I9" s="16">
+        <f>G9-F9</f>
+        <v>0.015390908965674018</v>
+      </c>
+      <c r="K9" s="73">
+        <v>146.322</v>
+      </c>
+      <c r="L9" s="74">
+        <f>DEGREES(ATAN(I9/H9))</f>
+        <v>19.628092303508957</v>
+      </c>
+      <c r="M9" s="75">
+        <f>6*SQRT(H9^2+I9^2)</f>
+        <v>0.27490849552311269</v>
+      </c>
+      <c r="N9" s="76">
+        <f>6/SQRT(5^2+C9^2)</f>
+        <v>0.27506931984611105</v>
+      </c>
+      <c r="O9" s="77">
+        <f>6/SQRT(17^2+B9^2)</f>
+        <v>0.2629348445100444</v>
+      </c>
+      <c r="P9"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="79"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" s="16">
+        <f>1/(2*PI()*K10*71.454*10^(-6))</f>
+        <v>12.177909915851149</v>
+      </c>
+      <c r="C10" s="16">
+        <f>2*PI()*K10*23.094*10^(-3)</f>
+        <v>26.539935235069031</v>
+      </c>
+      <c r="D10" s="16">
+        <f>17/(17^2+B10^2)</f>
+        <v>0.038874781796798728</v>
+      </c>
+      <c r="E10" s="16">
+        <f>5/(5^2+C10^2)</f>
+        <v>0.006855248499411686</v>
+      </c>
+      <c r="F10" s="16">
+        <f>B10/(17^2+B10^2)</f>
+        <v>0.027847858277634412</v>
+      </c>
+      <c r="G10" s="16">
+        <f>C10/(5^2+C10^2)</f>
+        <v>0.036387570238938065</v>
+      </c>
+      <c r="H10" s="16">
+        <f>E10+D10</f>
+        <v>0.045730030296210415</v>
+      </c>
+      <c r="I10" s="16">
+        <f>G10-F10</f>
+        <v>0.0085397119613036532</v>
+      </c>
+      <c r="K10" s="73">
+        <v>182.90299999999999</v>
+      </c>
+      <c r="L10" s="74">
+        <f>DEGREES(ATAN(I10/H10))</f>
+        <v>10.577687824773866</v>
+      </c>
+      <c r="M10" s="75">
+        <f>6*SQRT(H10^2+I10^2)</f>
+        <v>0.279123350234044</v>
+      </c>
+      <c r="N10" s="76">
+        <f>6/SQRT(5^2+C10^2)</f>
+        <v>0.22216612972225119</v>
+      </c>
+      <c r="O10" s="77">
+        <f>6/SQRT(17^2+B10^2)</f>
+        <v>0.28691996677540121</v>
+      </c>
+      <c r="P10"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="79"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" s="16">
+        <f>1/(2*PI()*K11*71.454*10^(-6))</f>
+        <v>10.148239768452017</v>
+      </c>
+      <c r="C11" s="16">
+        <f>2*PI()*K11*23.094*10^(-3)</f>
+        <v>31.84798032363544</v>
+      </c>
+      <c r="D11" s="16">
+        <f>17/(17^2+B11^2)</f>
+        <v>0.043368810592101362</v>
+      </c>
+      <c r="E11" s="16">
+        <f>5/(5^2+C11^2)</f>
+        <v>0.0048109588993122303</v>
+      </c>
+      <c r="F11" s="16">
+        <f>B11/(17^2+B11^2)</f>
+        <v>0.025889240491836833</v>
+      </c>
+      <c r="G11" s="16">
+        <f>C11/(5^2+C11^2)</f>
+        <v>0.030643864872622942</v>
+      </c>
+      <c r="H11" s="16">
+        <f>E11+D11</f>
+        <v>0.048179769491413595</v>
+      </c>
+      <c r="I11" s="16">
+        <f>G11-F11</f>
+        <v>0.0047546243807861099</v>
+      </c>
+      <c r="K11" s="73">
+        <v>219.48400000000001</v>
+      </c>
+      <c r="L11" s="74">
+        <f>DEGREES(ATAN(I11/H11))</f>
+        <v>5.6359900045415108</v>
+      </c>
+      <c r="M11" s="75">
+        <f>6*SQRT(H11^2+I11^2)</f>
+        <v>0.29048283784921292</v>
+      </c>
+      <c r="N11" s="76">
+        <f>6/SQRT(5^2+C11^2)</f>
+        <v>0.18611529779963831</v>
+      </c>
+      <c r="O11" s="77">
+        <f>6/SQRT(17^2+B11^2)</f>
+        <v>0.3030508772385227</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11" s="78"/>
+      <c r="R11" s="78"/>
+      <c r="S11" s="79"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="16">
+        <f>1/(2*PI()*K12*71.454*10^(-6))</f>
+        <v>8.6985138767609751</v>
+      </c>
+      <c r="C12" s="16">
+        <f>2*PI()*K12*23.094*10^(-3)</f>
+        <v>37.155880308320356</v>
+      </c>
+      <c r="D12" s="16">
+        <f>17/(17^2+B12^2)</f>
+        <v>0.04661823844039422</v>
+      </c>
+      <c r="E12" s="16">
+        <f>5/(5^2+C12^2)</f>
+        <v>0.0035573024181126314</v>
+      </c>
+      <c r="F12" s="16">
+        <f>B12/(17^2+B12^2)</f>
+        <v>0.023853493763760059</v>
+      </c>
+      <c r="G12" s="16">
+        <f>C12/(5^2+C12^2)</f>
+        <v>0.0264349405735783</v>
+      </c>
+      <c r="H12" s="16">
+        <f>E12+D12</f>
+        <v>0.050175540858506854</v>
+      </c>
+      <c r="I12" s="16">
+        <f>G12-F12</f>
+        <v>0.0025814468098182414</v>
+      </c>
+      <c r="K12" s="73">
+        <v>256.06400000000002</v>
+      </c>
+      <c r="L12" s="74">
+        <f>DEGREES(ATAN(I12/H12))</f>
+        <v>2.9451743357433435</v>
+      </c>
+      <c r="M12" s="75">
+        <f>6*SQRT(H12^2+I12^2)</f>
+        <v>0.30145141507500345</v>
+      </c>
+      <c r="N12" s="76">
+        <f>6/SQRT(5^2+C12^2)</f>
+        <v>0.16003929958110585</v>
+      </c>
+      <c r="O12" s="77">
+        <f>6/SQRT(17^2+B12^2)</f>
+        <v>0.31419894258389031</v>
+      </c>
+      <c r="P12"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="78"/>
+      <c r="S12" s="79"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="16">
+        <f>1/(2*PI()*K13*71.454*10^(-6))</f>
+        <v>7.61118849575056</v>
+      </c>
+      <c r="C13" s="16">
+        <f>2*PI()*K13*23.094*10^(-3)</f>
+        <v>42.463925396886751</v>
+      </c>
+      <c r="D13" s="16">
+        <f>17/(17^2+B13^2)</f>
+        <v>0.049001212562173317</v>
+      </c>
+      <c r="E13" s="16">
+        <f>5/(5^2+C13^2)</f>
+        <v>0.0027349530321552863</v>
+      </c>
+      <c r="F13" s="16">
+        <f>B13/(17^2+B13^2)</f>
+        <v>0.021938674431237728</v>
+      </c>
+      <c r="G13" s="16">
+        <f>C13/(5^2+C13^2)</f>
+        <v>0.023227368304286258</v>
+      </c>
+      <c r="H13" s="16">
+        <f>E13+D13</f>
+        <v>0.051736165594328601</v>
+      </c>
+      <c r="I13" s="16">
+        <f>G13-F13</f>
+        <v>0.0012886938730485298</v>
+      </c>
+      <c r="K13" s="73">
+        <v>292.64499999999998</v>
+      </c>
+      <c r="L13" s="74">
+        <f>DEGREES(ATAN(I13/H13))</f>
+        <v>1.4268829943275689</v>
+      </c>
+      <c r="M13" s="75">
+        <f>6*SQRT(H13^2+I13^2)</f>
+        <v>0.31051327869010703</v>
+      </c>
+      <c r="N13" s="76">
+        <f>6/SQRT(5^2+C13^2)</f>
+        <v>0.14032698183712947</v>
+      </c>
+      <c r="O13" s="77">
+        <f>6/SQRT(17^2+B13^2)</f>
+        <v>0.32212928097438281</v>
+      </c>
+      <c r="P13"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="79"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="16">
+        <f>1/(2*PI()*K14*71.454*10^(-6))</f>
+        <v>6.765513728723282</v>
+      </c>
+      <c r="C14" s="16">
+        <f>2*PI()*K14*23.094*10^(-3)</f>
+        <v>47.771825381571666</v>
+      </c>
+      <c r="D14" s="16">
+        <f>17/(17^2+B14^2)</f>
+        <v>0.05078080323889362</v>
+      </c>
+      <c r="E14" s="16">
+        <f>5/(5^2+C14^2)</f>
+        <v>0.0021671784889405227</v>
+      </c>
+      <c r="F14" s="16">
+        <f>B14/(17^2+B14^2)</f>
+        <v>0.02020930714519591</v>
+      </c>
+      <c r="G14" s="16">
+        <f>C14/(5^2+C14^2)</f>
+        <v>0.020706014468873001</v>
+      </c>
+      <c r="H14" s="16">
+        <f>E14+D14</f>
+        <v>0.052947981727834145</v>
+      </c>
+      <c r="I14" s="16">
+        <f>G14-F14</f>
+        <v>0.00049670732367709108</v>
+      </c>
+      <c r="K14" s="73">
+        <v>329.22500000000002</v>
+      </c>
+      <c r="L14" s="74">
+        <f>DEGREES(ATAN(I14/H14))</f>
+        <v>0.53747843776896664</v>
+      </c>
+      <c r="M14" s="75">
+        <f>6*SQRT(H14^2+I14^2)</f>
+        <v>0.31770186895860764</v>
+      </c>
+      <c r="N14" s="76">
+        <f>6/SQRT(5^2+C14^2)</f>
+        <v>0.12491471138489559</v>
+      </c>
+      <c r="O14" s="77">
+        <f>6/SQRT(17^2+B14^2)</f>
+        <v>0.3279265445546295</v>
+      </c>
+      <c r="P14"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="79"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="16">
+        <f>1/(2*PI()*K15*71.454*10^(-6))</f>
+        <v>6.0889549579255746</v>
+      </c>
+      <c r="C15" s="16">
+        <f>2*PI()*K15*23.094*10^(-3)</f>
+        <v>53.079870470138061</v>
+      </c>
+      <c r="D15" s="16">
+        <f>17/(17^2+B15^2)</f>
+        <v>0.052135185404292184</v>
+      </c>
+      <c r="E15" s="16">
+        <f>5/(5^2+C15^2)</f>
+        <v>0.0017590318772412032</v>
+      </c>
+      <c r="F15" s="16">
+        <f>B15/(17^2+B15^2)</f>
+        <v>0.018673458567637292</v>
+      </c>
+      <c r="G15" s="16">
+        <f>C15/(5^2+C15^2)</f>
+        <v>0.018673836839361371</v>
+      </c>
+      <c r="H15" s="16">
+        <f>E15+D15</f>
+        <v>0.053894217281533388</v>
+      </c>
+      <c r="I15" s="16">
+        <f>G15-F15</f>
+        <v>3.7827172407953191e-07</v>
+      </c>
+      <c r="K15" s="73">
+        <v>365.80599999999998</v>
+      </c>
+      <c r="L15" s="74">
+        <f>DEGREES(ATAN(I15/H15))</f>
+        <v>0.00040214654543215266</v>
+      </c>
+      <c r="M15" s="75">
+        <f>6*SQRT(H15^2+I15^2)</f>
+        <v>0.32336530369716532</v>
+      </c>
+      <c r="N15" s="76">
+        <f>6/SQRT(5^2+C15^2)</f>
+        <v>0.11253901330710459</v>
+      </c>
+      <c r="O15" s="77">
+        <f>6/SQRT(17^2+B15^2)</f>
+        <v>0.33227085642983906</v>
+      </c>
+      <c r="P15"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78"/>
+      <c r="S15" s="79"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="16">
+        <f>1/(2*PI()*K16*71.454*10^(-6))</f>
+        <v>5.5354080955371883</v>
+      </c>
+      <c r="C16" s="16">
+        <f>2*PI()*K16*23.094*10^(-3)</f>
+        <v>58.387915558704471</v>
+      </c>
+      <c r="D16" s="16">
+        <f>17/(17^2+B16^2)</f>
+        <v>0.053184709345643476</v>
+      </c>
+      <c r="E16" s="16">
+        <f>5/(5^2+C16^2)</f>
+        <v>0.0014559649162334135</v>
+      </c>
+      <c r="F16" s="16">
+        <f>B16/(17^2+B16^2)</f>
+        <v>0.017317592392392191</v>
+      </c>
+      <c r="G16" s="16">
+        <f>C16/(5^2+C16^2)</f>
+        <v>0.017002151317094556</v>
+      </c>
+      <c r="H16" s="16">
+        <f>E16+D16</f>
+        <v>0.054640674261876888</v>
+      </c>
+      <c r="I16" s="16">
+        <f>G16-F16</f>
+        <v>-0.00031544107529763582</v>
+      </c>
+      <c r="K16" s="73">
+        <v>402.387</v>
+      </c>
+      <c r="L16" s="74">
+        <f>DEGREES(ATAN(I16/H16))</f>
+        <v>-0.33076534589180584</v>
+      </c>
+      <c r="M16" s="75">
+        <f>6*SQRT(H16^2+I16^2)</f>
+        <v>0.32784950865774182</v>
+      </c>
+      <c r="N16" s="76">
+        <f>6/SQRT(5^2+C16^2)</f>
+        <v>0.1023862656652765</v>
+      </c>
+      <c r="O16" s="77">
+        <f>6/SQRT(17^2+B16^2)</f>
+        <v>0.33559863426448294</v>
+      </c>
+      <c r="P16"/>
+      <c r="Q16" s="78"/>
+      <c r="R16" s="78"/>
+      <c r="S16" s="79"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="16">
+        <f>1/(2*PI()*K17*71.454*10^(-6))</f>
+        <v>5.0741314434545703</v>
+      </c>
+      <c r="C17" s="16">
+        <f>2*PI()*K17*23.094*10^(-3)</f>
+        <v>63.695815543389386</v>
+      </c>
+      <c r="D17" s="16">
+        <f>17/(17^2+B17^2)</f>
+        <v>0.054011667362431938</v>
+      </c>
+      <c r="E17" s="16">
+        <f>5/(5^2+C17^2)</f>
+        <v>0.0012248426752715879</v>
+      </c>
+      <c r="F17" s="16">
+        <f>B17/(17^2+B17^2)</f>
+        <v>0.01612131174571323</v>
+      </c>
+      <c r="G17" s="16">
+        <f>C17/(5^2+C17^2)</f>
+        <v>0.015603470622754127</v>
+      </c>
+      <c r="H17" s="16">
+        <f>E17+D17</f>
+        <v>0.055236510037703523</v>
+      </c>
+      <c r="I17" s="16">
+        <f>G17-F17</f>
+        <v>-0.00051784112295910276</v>
+      </c>
+      <c r="K17" s="73">
+        <v>438.96699999999998</v>
+      </c>
+      <c r="L17" s="74">
+        <f>DEGREES(ATAN(I17/H17))</f>
+        <v>-0.53713099527500729</v>
+      </c>
+      <c r="M17" s="75">
+        <f>6*SQRT(H17^2+I17^2)</f>
+        <v>0.33143362415521782</v>
+      </c>
+      <c r="N17" s="76">
+        <f>6/SQRT(5^2+C17^2)</f>
+        <v>0.093908824196426988</v>
+      </c>
+      <c r="O17" s="77">
+        <f>6/SQRT(17^2+B17^2)</f>
+        <v>0.33819764714173994</v>
+      </c>
+      <c r="P17"/>
+      <c r="Q17" s="78"/>
+      <c r="R17" s="78"/>
+      <c r="S17" s="79"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="16">
+        <f>1/(2*PI()*K18*71.454*10^(-6))</f>
+        <v>4.6838095362380292</v>
+      </c>
+      <c r="C18" s="16">
+        <f>2*PI()*K18*23.094*10^(-3)</f>
+        <v>69.003860631955789</v>
+      </c>
+      <c r="D18" s="16">
+        <f>17/(17^2+B18^2)</f>
+        <v>0.054673266297473336</v>
+      </c>
+      <c r="E18" s="16">
+        <f>5/(5^2+C18^2)</f>
+        <v>0.001044597462840592</v>
+      </c>
+      <c r="F18" s="16">
+        <f>B18/(17^2+B18^2)</f>
+        <v>0.015063480356552167</v>
+      </c>
+      <c r="G18" s="16">
+        <f>C18/(5^2+C18^2)</f>
+        <v>0.014416251548469367</v>
+      </c>
+      <c r="H18" s="16">
+        <f>E18+D18</f>
+        <v>0.055717863760313929</v>
+      </c>
+      <c r="I18" s="16">
+        <f>G18-F18</f>
+        <v>-0.00064722880808280002</v>
+      </c>
+      <c r="K18" s="73">
+        <v>475.548</v>
+      </c>
+      <c r="L18" s="74">
+        <f>DEGREES(ATAN(I18/H18))</f>
+        <v>-0.66552823014943396</v>
+      </c>
+      <c r="M18" s="75">
+        <f>6*SQRT(H18^2+I18^2)</f>
+        <v>0.3343297367826335</v>
+      </c>
+      <c r="N18" s="76">
+        <f>6/SQRT(5^2+C18^2)</f>
+        <v>0.086724285713128027</v>
+      </c>
+      <c r="O18" s="77">
+        <f>6/SQRT(17^2+B18^2)</f>
+        <v>0.34026266555577328</v>
+      </c>
+      <c r="P18"/>
+      <c r="Q18" s="78"/>
+      <c r="R18" s="78"/>
+      <c r="S18" s="79"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="16">
+        <f>1/(2*PI()*K19*71.454*10^(-6))</f>
+        <v>4.3492569383804875</v>
+      </c>
+      <c r="C19" s="16">
+        <f>2*PI()*K19*23.094*10^(-3)</f>
+        <v>74.311760616640711</v>
+      </c>
+      <c r="D19" s="16">
+        <f>17/(17^2+B19^2)</f>
+        <v>0.055209855990205142</v>
+      </c>
+      <c r="E19" s="16">
+        <f>5/(5^2+C19^2)</f>
+        <v>0.00090134950239478373</v>
+      </c>
+      <c r="F19" s="16">
+        <f>B19/(17^2+B19^2)</f>
+        <v>0.01412481466072866</v>
+      </c>
+      <c r="G19" s="16">
+        <f>C19/(5^2+C19^2)</f>
+        <v>0.013396173690777878</v>
+      </c>
+      <c r="H19" s="16">
+        <f>E19+D19</f>
+        <v>0.056111205492599923</v>
+      </c>
+      <c r="I19" s="16">
+        <f>G19-F19</f>
+        <v>-0.00072864096995078204</v>
+      </c>
+      <c r="K19" s="73">
+        <v>512.12800000000004</v>
+      </c>
+      <c r="L19" s="74">
+        <f>DEGREES(ATAN(I19/H19))</f>
+        <v>-0.743981627350082</v>
+      </c>
+      <c r="M19" s="75">
+        <f>6*SQRT(H19^2+I19^2)</f>
+        <v>0.33669561740814391</v>
+      </c>
+      <c r="N19" s="76">
+        <f>6/SQRT(5^2+C19^2)</f>
+        <v>0.080558776165247453</v>
+      </c>
+      <c r="O19" s="77">
+        <f>6/SQRT(17^2+B19^2)</f>
+        <v>0.3419283392111987</v>
+      </c>
+      <c r="P19"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="78"/>
+      <c r="S19" s="79"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="16">
+        <f>1/(2*PI()*K20*71.454*10^(-6))</f>
+        <v>4.0593033052837164</v>
+      </c>
+      <c r="C20" s="16">
+        <f>2*PI()*K20*23.094*10^(-3)</f>
+        <v>79.619805705207099</v>
+      </c>
+      <c r="D20" s="16">
+        <f>17/(17^2+B20^2)</f>
+        <v>0.055650499067139682</v>
+      </c>
+      <c r="E20" s="16">
+        <f>5/(5^2+C20^2)</f>
+        <v>0.00078563069386902002</v>
+      </c>
+      <c r="F20" s="16">
+        <f>B20/(17^2+B20^2)</f>
+        <v>0.013288367929642853</v>
+      </c>
+      <c r="G20" s="16">
+        <f>C20/(5^2+C20^2)</f>
+        <v>0.012510352640379682</v>
+      </c>
+      <c r="H20" s="16">
+        <f>E20+D20</f>
+        <v>0.056436129761008702</v>
+      </c>
+      <c r="I20" s="16">
+        <f>G20-F20</f>
+        <v>-0.00077801528926317066</v>
+      </c>
+      <c r="K20" s="73">
+        <v>548.70899999999995</v>
+      </c>
+      <c r="L20" s="74">
+        <f>DEGREES(ATAN(I20/H20))</f>
+        <v>-0.78981618812390275</v>
+      </c>
+      <c r="M20" s="75">
+        <f>6*SQRT(H20^2+I20^2)</f>
+        <v>0.33864895364802566</v>
+      </c>
+      <c r="N20" s="76">
+        <f>6/SQRT(5^2+C20^2)</f>
+        <v>0.075209979363492344</v>
+      </c>
+      <c r="O20" s="77">
+        <f>6/SQRT(17^2+B20^2)</f>
+        <v>0.34329013337349196</v>
+      </c>
+      <c r="P20"/>
+      <c r="Q20" s="78"/>
+      <c r="R20" s="78"/>
+      <c r="S20" s="79"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="16">
+        <f>1/(2*PI()*K21*71.454*10^(-6))</f>
+        <v>3.80559424787528</v>
+      </c>
+      <c r="C21" s="16">
+        <f>2*PI()*K21*23.094*10^(-3)</f>
+        <v>84.927850793773501</v>
+      </c>
+      <c r="D21" s="16">
+        <f>17/(17^2+B21^2)</f>
+        <v>0.056016400730749955</v>
+      </c>
+      <c r="E21" s="16">
+        <f>5/(5^2+C21^2)</f>
+        <v>0.00069082339379713132</v>
+      </c>
+      <c r="F21" s="16">
+        <f>B21/(17^2+B21^2)</f>
+        <v>0.012539746612212861</v>
+      </c>
+      <c r="G21" s="16">
+        <f>C21/(5^2+C21^2)</f>
+        <v>0.011734029222650202</v>
+      </c>
+      <c r="H21" s="16">
+        <f>E21+D21</f>
+        <v>0.056707224124547088</v>
+      </c>
+      <c r="I21" s="16">
+        <f>G21-F21</f>
+        <v>-0.00080571738956265911</v>
+      </c>
+      <c r="K21" s="73">
+        <v>585.28999999999996</v>
+      </c>
+      <c r="L21" s="74">
+        <f>DEGREES(ATAN(I21/H21))</f>
+        <v>-0.81402502909831753</v>
+      </c>
+      <c r="M21" s="75">
+        <f>6*SQRT(H21^2+I21^2)</f>
+        <v>0.34027768681364418</v>
+      </c>
+      <c r="N21" s="76">
+        <f>6/SQRT(5^2+C21^2)</f>
+        <v>0.070526083368774611</v>
+      </c>
+      <c r="O21" s="77">
+        <f>6/SQRT(17^2+B21^2)</f>
+        <v>0.34441684954913698</v>
+      </c>
+      <c r="P21"/>
+      <c r="Q21" s="78"/>
+      <c r="R21" s="78"/>
+      <c r="S21" s="79"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="16">
+        <f>1/(2*PI()*K22*71.454*10^(-6))</f>
+        <v>3.5817393624695226</v>
+      </c>
+      <c r="C22" s="16">
+        <f>2*PI()*K22*23.094*10^(-3)</f>
+        <v>90.235750778458424</v>
+      </c>
+      <c r="D22" s="16">
+        <f>17/(17^2+B22^2)</f>
+        <v>0.056323309099129276</v>
+      </c>
+      <c r="E22" s="16">
+        <f>5/(5^2+C22^2)</f>
+        <v>0.00061218312604172803</v>
+      </c>
+      <c r="F22" s="16">
+        <f>B22/(17^2+B22^2)</f>
+        <v>0.011866789013228773</v>
+      </c>
+      <c r="G22" s="16">
+        <f>C22/(5^2+C22^2)</f>
+        <v>0.011048160798455794</v>
+      </c>
+      <c r="H22" s="16">
+        <f>E22+D22</f>
+        <v>0.056935492225171004</v>
+      </c>
+      <c r="I22" s="16">
+        <f>G22-F22</f>
+        <v>-0.00081862821477297898</v>
+      </c>
+      <c r="K22" s="73">
+        <v>621.87</v>
+      </c>
+      <c r="L22" s="74">
+        <f>DEGREES(ATAN(I22/H22))</f>
+        <v>-0.8237517247349383</v>
+      </c>
+      <c r="M22" s="75">
+        <f>6*SQRT(H22^2+I22^2)</f>
+        <v>0.34164826265437837</v>
+      </c>
+      <c r="N22" s="76">
+        <f>6/SQRT(5^2+C22^2)</f>
+        <v>0.06639065075370508</v>
+      </c>
+      <c r="O22" s="77">
+        <f>6/SQRT(17^2+B22^2)</f>
+        <v>0.34535907380142722</v>
+      </c>
+      <c r="P22"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="79"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="16">
+        <f>1/(2*PI()*K23*71.454*10^(-6))</f>
+        <v>3.3827517269150205</v>
+      </c>
+      <c r="C23" s="16">
+        <f>2*PI()*K23*23.094*10^(-3)</f>
+        <v>95.543795867024841</v>
+      </c>
+      <c r="D23" s="16">
+        <f>17/(17^2+B23^2)</f>
+        <v>0.056583110529569949</v>
+      </c>
+      <c r="E23" s="16">
+        <f>5/(5^2+C23^2)</f>
+        <v>0.00054623216581570276</v>
+      </c>
+      <c r="F23" s="16">
+        <f>B23/(17^2+B23^2)</f>
+        <v>0.011259212638713307</v>
+      </c>
+      <c r="G23" s="16">
+        <f>C23/(5^2+C23^2)</f>
+        <v>0.010437818909339673</v>
+      </c>
+      <c r="H23" s="16">
+        <f>E23+D23</f>
+        <v>0.057129342695385651</v>
+      </c>
+      <c r="I23" s="16">
+        <f>G23-F23</f>
+        <v>-0.00082139372937363453</v>
+      </c>
+      <c r="K23" s="73">
+        <v>658.45100000000002</v>
+      </c>
+      <c r="L23" s="74">
+        <f>DEGREES(ATAN(I23/H23))</f>
+        <v>-0.82372996550052724</v>
+      </c>
+      <c r="M23" s="75">
+        <f>6*SQRT(H23^2+I23^2)</f>
+        <v>0.34281148382275184</v>
+      </c>
+      <c r="N23" s="76">
+        <f>6/SQRT(5^2+C23^2)</f>
+        <v>0.062712611123067266</v>
+      </c>
+      <c r="O23" s="77">
+        <f>6/SQRT(17^2+B23^2)</f>
+        <v>0.34615467293109087</v>
+      </c>
+      <c r="P23"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="79"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="16">
+        <f>1/(2*PI()*K24*71.454*10^(-6))</f>
+        <v>3.204714980107251</v>
+      </c>
+      <c r="C24" s="16">
+        <f>2*PI()*K24*23.094*10^(-3)</f>
+        <v>100.85169585170974</v>
+      </c>
+      <c r="D24" s="16">
+        <f>17/(17^2+B24^2)</f>
+        <v>0.056804854301289238</v>
+      </c>
+      <c r="E24" s="16">
+        <f>5/(5^2+C24^2)</f>
+        <v>0.00049038528271934086</v>
+      </c>
+      <c r="F24" s="16">
+        <f>B24/(17^2+B24^2)</f>
+        <v>0.010708433383655968</v>
+      </c>
+      <c r="G24" s="16">
+        <f>C24/(5^2+C24^2)</f>
+        <v>0.0098912374765931319</v>
+      </c>
+      <c r="H24" s="16">
+        <f>E24+D24</f>
+        <v>0.057295239584008582</v>
+      </c>
+      <c r="I24" s="16">
+        <f>G24-F24</f>
+        <v>-0.00081719590706283603</v>
+      </c>
+      <c r="K24" s="73">
+        <v>695.03099999999995</v>
+      </c>
+      <c r="L24" s="74">
+        <f>DEGREES(ATAN(I24/H24))</f>
+        <v>-0.81714820016332856</v>
+      </c>
+      <c r="M24" s="75">
+        <f>6*SQRT(H24^2+I24^2)</f>
+        <v>0.34380640246077543</v>
+      </c>
+      <c r="N24" s="76">
+        <f>6/SQRT(5^2+C24^2)</f>
+        <v>0.059420316690331217</v>
+      </c>
+      <c r="O24" s="77">
+        <f>6/SQRT(17^2+B24^2)</f>
+        <v>0.34683228315429965</v>
+      </c>
+      <c r="P24"/>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="79"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" s="16">
+        <f>1/(2*PI()*K25*71.454*10^(-6))</f>
+        <v>3.0444774789627873</v>
+      </c>
+      <c r="C25" s="16">
+        <f>2*PI()*K25*23.094*10^(-3)</f>
+        <v>106.15974094027612</v>
+      </c>
+      <c r="D25" s="16">
+        <f>17/(17^2+B25^2)</f>
+        <v>0.056995560857711083</v>
+      </c>
+      <c r="E25" s="16">
+        <f>5/(5^2+C25^2)</f>
+        <v>0.00044267803723096517</v>
+      </c>
+      <c r="F25" s="16">
+        <f>B25/(17^2+B25^2)</f>
+        <v>0.010207158907773786</v>
+      </c>
+      <c r="G25" s="16">
+        <f>C25/(5^2+C25^2)</f>
+        <v>0.0093989171504778347</v>
+      </c>
+      <c r="H25" s="16">
+        <f>E25+D25</f>
+        <v>0.057438238894942047</v>
+      </c>
+      <c r="I25" s="16">
+        <f>G25-F25</f>
+        <v>-0.00080824175729595112</v>
+      </c>
+      <c r="K25" s="80">
+        <v>731.61199999999997</v>
+      </c>
+      <c r="L25" s="81">
+        <f>DEGREES(ATAN(I25/H25))</f>
+        <v>-0.80618393396292942</v>
+      </c>
+      <c r="M25" s="82">
+        <f>6*SQRT(H25^2+I25^2)</f>
+        <v>0.34466355118472292</v>
+      </c>
+      <c r="N25" s="83">
+        <f>6/SQRT(5^2+C25^2)</f>
+        <v>0.056456017111225172</v>
+      </c>
+      <c r="O25" s="84">
+        <f>6/SQRT(17^2+B25^2)</f>
+        <v>0.34741399196970946</v>
+      </c>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="85"/>
+      <c r="R25" s="85"/>
+      <c r="S25" s="86"/>
+    </row>
+    <row r="27" ht="14.25"/>
+    <row r="28" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:S2"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="Q5:S5"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
     <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -5386,530 +7022,530 @@
   </cols>
   <sheetData>
     <row r="2" ht="29.399999999999999" customHeight="1">
-      <c r="B2" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="52"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
+      <c r="B2" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="90"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
     </row>
     <row r="3">
-      <c r="B3" s="57"/>
-      <c r="C3" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="58" t="s">
+      <c r="B3" s="95"/>
+      <c r="C3" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="54"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
     </row>
     <row r="4">
-      <c r="B4" s="57"/>
-      <c r="C4" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="58" t="s">
+      <c r="B4" s="95"/>
+      <c r="C4" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="99"/>
+      <c r="E4" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="62" t="s">
+      <c r="J4" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="N4" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="64" t="s">
+      <c r="M4" s="101" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="101" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="64" t="s">
+      <c r="P4" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="64" t="s">
+      <c r="Q4" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="R4" s="102" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="65">
+      <c r="B5" s="103">
         <v>1</v>
       </c>
-      <c r="C5" s="66">
+      <c r="C5" s="104">
         <v>30</v>
       </c>
-      <c r="D5" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="66">
+      <c r="D5" s="104" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="104" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="104">
         <v>6.0170000000000003</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="104">
         <v>0.19900000000000001</v>
       </c>
-      <c r="I5" s="67">
+      <c r="I5" s="105">
         <v>0</v>
       </c>
-      <c r="J5" s="66">
+      <c r="J5" s="104">
         <v>0.20000000000000001</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="105">
         <v>0</v>
       </c>
-      <c r="M5" s="63">
+      <c r="M5" s="101">
         <v>0.28199999999999997</v>
       </c>
-      <c r="N5" s="63">
+      <c r="N5" s="101">
         <v>8.5099999999999998</v>
       </c>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
     </row>
     <row r="6">
-      <c r="B6" s="68">
+      <c r="B6" s="106">
         <v>2</v>
       </c>
-      <c r="C6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="70">
+      <c r="C6" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="108">
         <v>71.453999999999994</v>
       </c>
-      <c r="G6" s="69">
+      <c r="G6" s="107">
         <v>6.0039999999999996</v>
       </c>
-      <c r="H6" s="69">
+      <c r="H6" s="107">
         <v>0.053600000000000002</v>
       </c>
-      <c r="I6" s="70">
+      <c r="I6" s="108">
         <v>-88.519000000000005</v>
       </c>
-      <c r="J6" s="69">
+      <c r="J6" s="107">
         <v>0.053600000000000002</v>
       </c>
-      <c r="K6" s="70">
+      <c r="K6" s="108">
         <v>-90</v>
       </c>
-      <c r="M6" s="63">
+      <c r="M6" s="101">
         <v>0.075819999999999999</v>
       </c>
-      <c r="N6" s="63">
+      <c r="N6" s="101">
         <v>8.4909999999999997</v>
       </c>
-      <c r="O6" s="71">
+      <c r="O6" s="109">
         <v>12.56</v>
       </c>
-      <c r="P6" s="71">
+      <c r="P6" s="109">
         <v>25.109999999999999</v>
       </c>
-      <c r="Q6" s="71">
+      <c r="Q6" s="109">
         <v>0</v>
       </c>
-      <c r="R6" s="71">
+      <c r="R6" s="109">
         <v>25.52</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="68">
+      <c r="B7" s="106">
         <v>3</v>
       </c>
-      <c r="C7" s="69">
+      <c r="C7" s="107">
         <v>30</v>
       </c>
-      <c r="D7" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="70">
+      <c r="D7" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="108">
         <v>71.453999999999994</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="107">
         <v>6.0004999999999997</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="107">
         <v>0.051799999999999999</v>
       </c>
-      <c r="I7" s="70">
+      <c r="I7" s="108">
         <v>-74.896000000000001</v>
       </c>
-      <c r="J7" s="69">
+      <c r="J7" s="107">
         <v>0.051799999999999999</v>
       </c>
-      <c r="K7" s="70">
+      <c r="K7" s="108">
         <v>-75</v>
       </c>
-      <c r="M7" s="63">
+      <c r="M7" s="101">
         <v>0.073219999999999993</v>
       </c>
-      <c r="N7" s="63">
+      <c r="N7" s="101">
         <v>8.4860000000000007</v>
       </c>
-      <c r="O7" s="71">
+      <c r="O7" s="109">
         <v>50.189999999999998</v>
       </c>
-      <c r="P7" s="71">
+      <c r="P7" s="109">
         <v>61.880000000000003</v>
       </c>
-      <c r="Q7" s="71">
+      <c r="Q7" s="109">
         <v>100.56</v>
       </c>
-      <c r="R7" s="71">
+      <c r="R7" s="109">
         <v>125.70999999999999</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="72">
+      <c r="B8" s="110">
         <v>4</v>
       </c>
-      <c r="C8" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="73">
+      <c r="C8" s="111" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="111">
         <v>5</v>
       </c>
-      <c r="E8" s="73">
+      <c r="E8" s="111">
         <v>23.094000000000001</v>
       </c>
-      <c r="F8" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="73">
+      <c r="F8" s="112" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="111">
         <v>5.9909999999999997</v>
       </c>
-      <c r="H8" s="73">
+      <c r="H8" s="111">
         <v>1.0397000000000001</v>
       </c>
-      <c r="I8" s="74">
+      <c r="I8" s="112">
         <v>30.713000000000001</v>
       </c>
-      <c r="J8" s="73">
+      <c r="J8" s="111">
         <v>1.0389999999999999</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="112">
         <v>30.699999999999999</v>
       </c>
-      <c r="M8" s="63">
+      <c r="M8" s="101">
         <v>1.4702999999999999</v>
       </c>
-      <c r="N8" s="63">
+      <c r="N8" s="101">
         <v>8.4719999999999995</v>
       </c>
-      <c r="O8" s="71">
+      <c r="O8" s="109">
         <v>50.240000000000002</v>
       </c>
-      <c r="P8" s="71">
+      <c r="P8" s="109">
         <v>54.549999999999997</v>
       </c>
-      <c r="Q8" s="71">
+      <c r="Q8" s="109">
         <v>50.210000000000001</v>
       </c>
-      <c r="R8" s="71">
+      <c r="R8" s="109">
         <v>75.469999999999999</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="72">
+      <c r="B9" s="110">
         <v>5</v>
       </c>
-      <c r="C9" s="73">
+      <c r="C9" s="111">
         <v>30</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D9" s="111">
         <v>5</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="111">
         <v>23.094000000000001</v>
       </c>
-      <c r="F9" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="73">
+      <c r="F9" s="112" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="111">
         <v>5.9980000000000002</v>
       </c>
-      <c r="H9" s="73">
+      <c r="H9" s="111">
         <v>0.17100000000000001</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="112">
         <v>4.9080000000000004</v>
       </c>
-      <c r="J9" s="73">
+      <c r="J9" s="111">
         <v>0.17100000000000001</v>
       </c>
-      <c r="K9" s="74">
+      <c r="K9" s="112">
         <v>4.7199999999999998</v>
       </c>
-      <c r="M9" s="63">
+      <c r="M9" s="101">
         <v>0.24223</v>
       </c>
-      <c r="N9" s="63">
+      <c r="N9" s="101">
         <v>8.4831000000000003</v>
       </c>
-      <c r="O9" s="71">
+      <c r="O9" s="109">
         <v>50.264000000000003</v>
       </c>
-      <c r="P9" s="71">
+      <c r="P9" s="109">
         <v>50.951999999999998</v>
       </c>
-      <c r="Q9" s="71">
+      <c r="Q9" s="109">
         <v>50.210000000000001</v>
       </c>
-      <c r="R9" s="71">
+      <c r="R9" s="109">
         <v>75.430000000000007</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="75">
+      <c r="B10" s="113">
         <v>6</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="114">
         <v>30</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="114">
         <v>5</v>
       </c>
-      <c r="E10" s="76">
+      <c r="E10" s="114">
         <v>23.094000000000001</v>
       </c>
-      <c r="F10" s="77">
+      <c r="F10" s="115">
         <v>71.453999999999994</v>
       </c>
-      <c r="G10" s="76">
+      <c r="G10" s="114">
         <v>6.0010000000000003</v>
       </c>
-      <c r="H10" s="76">
+      <c r="H10" s="114">
         <v>0.052400000000000002</v>
       </c>
-      <c r="I10" s="77">
+      <c r="I10" s="115">
         <v>-72.158000000000001</v>
       </c>
-      <c r="J10" s="76">
+      <c r="J10" s="114">
         <v>0.052400000000000002</v>
       </c>
-      <c r="K10" s="77">
+      <c r="K10" s="115">
         <v>-72.209000000000003</v>
       </c>
-      <c r="M10" s="63">
+      <c r="M10" s="101">
         <v>0.074139999999999998</v>
       </c>
-      <c r="N10" s="63">
+      <c r="N10" s="101">
         <v>8</v>
       </c>
-      <c r="O10" s="71">
+      <c r="O10" s="109">
         <v>38.670000000000002</v>
       </c>
-      <c r="P10" s="71">
+      <c r="P10" s="109">
         <v>50.270000000000003</v>
       </c>
-      <c r="Q10" s="71">
+      <c r="Q10" s="109">
         <v>50.200000000000003</v>
       </c>
-      <c r="R10" s="71">
+      <c r="R10" s="109">
         <v>75.459999999999994</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="68">
+      <c r="B11" s="106">
         <v>7</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="107">
         <v>30</v>
       </c>
-      <c r="D11" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="70">
+      <c r="D11" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="108">
         <v>71.453999999999994</v>
       </c>
-      <c r="G11" s="69">
+      <c r="G11" s="107">
         <v>5.9997999999999996</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="107">
         <v>0.20699999999999999</v>
       </c>
-      <c r="I11" s="70">
+      <c r="I11" s="108">
         <v>-16.594000000000001</v>
       </c>
-      <c r="J11" s="69">
+      <c r="J11" s="107">
         <v>0.20699999999999999</v>
       </c>
-      <c r="K11" s="70">
+      <c r="K11" s="108">
         <v>-16.577000000000002</v>
       </c>
-      <c r="M11" s="63">
+      <c r="M11" s="101">
         <v>0.29293000000000002</v>
       </c>
-      <c r="N11" s="63">
+      <c r="N11" s="101">
         <v>8.4850010000000005</v>
       </c>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
+      <c r="O11" s="94"/>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="94"/>
     </row>
     <row r="12">
-      <c r="B12" s="72">
+      <c r="B12" s="110">
         <v>8</v>
       </c>
-      <c r="C12" s="73">
+      <c r="C12" s="111">
         <v>30</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D12" s="111">
         <v>5</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="111">
         <v>23.094000000000001</v>
       </c>
-      <c r="F12" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="73">
+      <c r="F12" s="112" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="111">
         <v>5.9983000000000004</v>
       </c>
-      <c r="H12" s="73">
+      <c r="H12" s="111">
         <v>1.216</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="112">
         <v>25.327000000000002</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="111">
         <v>1.2170000000000001</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="112">
         <v>25.324999999999999</v>
       </c>
-      <c r="M12" s="63">
+      <c r="M12" s="101">
         <v>1.7196</v>
       </c>
-      <c r="N12" s="63">
+      <c r="N12" s="101">
         <v>8.4828600000000005</v>
       </c>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="56"/>
+      <c r="O12" s="94"/>
+      <c r="P12" s="94"/>
+      <c r="Q12" s="94"/>
+      <c r="R12" s="94"/>
     </row>
     <row r="13">
-      <c r="B13" s="78">
+      <c r="B13" s="116">
         <v>9</v>
       </c>
-      <c r="C13" s="79">
+      <c r="C13" s="117">
         <v>30</v>
       </c>
-      <c r="D13" s="79">
+      <c r="D13" s="117">
         <v>5</v>
       </c>
-      <c r="E13" s="79">
+      <c r="E13" s="117">
         <v>23.094000000000001</v>
       </c>
-      <c r="F13" s="80">
+      <c r="F13" s="118">
         <v>71.453999999999994</v>
       </c>
-      <c r="G13" s="79">
+      <c r="G13" s="117">
         <v>5.9989999999999997</v>
       </c>
-      <c r="H13" s="79">
+      <c r="H13" s="117">
         <v>1.0269999999999999</v>
       </c>
-      <c r="I13" s="80">
+      <c r="I13" s="118">
         <v>27.254999999999999</v>
       </c>
-      <c r="J13" s="79">
+      <c r="J13" s="117">
         <v>1.0269999999999999</v>
       </c>
-      <c r="K13" s="80">
+      <c r="K13" s="118">
         <v>27.254000000000001</v>
       </c>
-      <c r="M13" s="63">
+      <c r="M13" s="101">
         <v>1.4521999999999999</v>
       </c>
-      <c r="N13" s="63">
+      <c r="N13" s="101">
         <v>8.4841999999999995</v>
       </c>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>